<commit_message>
Updated sprint 2 date range
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint2/plan.xlsx
+++ b/sprint_backlog/sprint2/plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ajg\Documents (D)\Repositories\CSCC01\Team5\sprint_backlog\sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajg\Documents\Repositories\CSCC01\Team5\sprint_backlog\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21009789-9AE7-4DD8-88CF-696CE64AAF52}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A46B84A-3B71-425F-8D4E-389430770317}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
     <t>T9, T10, (T11, T13)</t>
   </si>
   <si>
-    <t>Sprint 2 Plan (Oct 23 - Oct 27)</t>
+    <t>Sprint 2 Plan (Oct 24 - Oct 28)</t>
   </si>
 </sst>
 </file>
@@ -307,7 +307,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,7 +316,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,16 +706,16 @@
       <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="1025" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.3046875" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" customWidth="1"/>
+    <col min="3" max="3" width="16.53515625" customWidth="1"/>
+    <col min="4" max="4" width="11.53515625" customWidth="1"/>
+    <col min="5" max="1025" width="8.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>42</v>
       </c>
@@ -730,7 +730,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -743,7 +743,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -772,7 +772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -795,8 +795,8 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -824,7 +824,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -853,8 +853,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -876,8 +876,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -903,8 +903,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -922,8 +922,8 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
@@ -939,8 +939,8 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -958,8 +958,8 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -977,7 +977,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Updated sprint 2 plan
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint2/plan.xlsx
+++ b/sprint_backlog/sprint2/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ajg\Documents (D)\Repositories\CSCC01\Team5\sprint_backlog\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21009789-9AE7-4DD8-88CF-696CE64AAF52}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477393D8-7BC4-4CE2-A8C5-D54F63B1FAF6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,7 +316,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,7 +703,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+      <selection activeCell="E8" sqref="E8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,17 +786,17 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -854,7 +854,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -862,10 +862,14 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
@@ -877,7 +881,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -885,14 +889,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="3">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
@@ -904,7 +904,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -923,7 +923,7 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
@@ -940,7 +940,7 @@
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -959,7 +959,7 @@
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">

</xml_diff>